<commit_message>
add feature for student review and integrate flask api for correction and feedback model
</commit_message>
<xml_diff>
--- a/public/formatExcel/QuestionImportFormat.xlsx
+++ b/public/formatExcel/QuestionImportFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AGILL\POLITEKNIK NEGERI JAKARTA\MATA KULIAH\SEMESTER 8\KODE\LMS_GRAFIKA_AES\public\formatExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A03348-36CD-4452-9B1F-349B1597B40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD92C443-01EE-4FA8-967E-9206840702B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D2AB067-9465-403A-B7D7-A94F9C72CB8D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>No.</t>
   </si>
@@ -75,6 +75,11 @@
   <si>
     <t>Jawaban Benar
 (untuk multiple A/B/C/D/E)</t>
+  </si>
+  <si>
+    <t>Jenis tipe soal
+(untuk essay
+terbatas/bebas)</t>
   </si>
 </sst>
 </file>
@@ -449,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEFC0B-6FD7-4307-9494-B77D4B0A9A63}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,9 +473,10 @@
     <col min="9" max="9" width="30.42578125" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="33.140625" customWidth="1"/>
+    <col min="12" max="12" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,8 +510,11 @@
       <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -518,7 +527,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>

</xml_diff>